<commit_message>
add guild data module
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Guild.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Guild.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="60">
   <si>
     <t>Id</t>
   </si>
@@ -241,6 +241,18 @@
   <si>
     <t>GuildBoss</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>工会ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>object</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GuilID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -654,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -991,6 +1003,38 @@
       </c>
       <c r="J10" s="3" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify bug of the objectsavemodule
Former-commit-id: af025c0f316d611c41069661f893dd6873dbf215 [formerly b028e7c4feceabea0d708154ee064a012c4f100f]
Former-commit-id: 8ea6c09356913f6bf55226be29f32bd61c9cea41
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Guild.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Guild.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -265,6 +265,10 @@
       </rPr>
       <t>ameID</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Online</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1393,7 +1397,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1469,7 +1473,7 @@
         <v>38</v>
       </c>
       <c r="S1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="T1" t="s">
         <v>40</v>
@@ -1492,7 +1496,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>

</xml_diff>